<commit_message>
fix: 3T segmentation regions now consistent
- 3T segmentation regions were swapped w.r.t. the 1.5T segmentation.
  This has now been corrected
</commit_message>
<xml_diff>
--- a/data/3T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
+++ b/data/3T/thermometry_analysis_Method.REGIONWISE_BOOTSTRAP.xlsx
@@ -480,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>9.992453778919103</v>
+        <v>10.10857839943257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.287811754187309</v>
+        <v>0.3251935834333333</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -500,10 +500,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>10.10857839943257</v>
+        <v>9.992453778919103</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3251935834333333</v>
+        <v>0.287811754187309</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -520,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>11.23206565283856</v>
+        <v>10.9301682871816</v>
       </c>
       <c r="E4" t="n">
-        <v>0.344013092057436</v>
+        <v>0.3418071732138103</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -540,10 +540,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>10.9301682871816</v>
+        <v>11.23206565283856</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3418071732138103</v>
+        <v>0.344013092057436</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -560,10 +560,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>12.36835486658175</v>
+        <v>11.56845410765602</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3843332476524426</v>
+        <v>0.3383422763088164</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -580,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>11.56845410765602</v>
+        <v>12.36835486658175</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3383422763088164</v>
+        <v>0.3843332476524426</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -600,10 +600,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>13.2399779545139</v>
+        <v>12.20114075165322</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4783879085873868</v>
+        <v>0.3173074193737433</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -620,10 +620,10 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>12.20114075165322</v>
+        <v>13.2399779545139</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3173074193737433</v>
+        <v>0.4783879085873868</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -640,10 +640,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>14.32611534610258</v>
+        <v>12.98811862555542</v>
       </c>
       <c r="E10" t="n">
-        <v>0.4698530346716841</v>
+        <v>0.3437019179304072</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -660,10 +660,10 @@
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>12.98811862555542</v>
+        <v>14.32611534610258</v>
       </c>
       <c r="E11" t="n">
-        <v>0.3437019179304072</v>
+        <v>0.4698530346716841</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -680,10 +680,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>15.28532866917971</v>
+        <v>13.95986055928058</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4905165895958741</v>
+        <v>0.3993950526869441</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -700,10 +700,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>13.95986055928058</v>
+        <v>15.28532866917971</v>
       </c>
       <c r="E13" t="n">
-        <v>0.3993950526869441</v>
+        <v>0.4905165895958741</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -720,10 +720,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>15.92520679514612</v>
+        <v>14.72354656194007</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4945554042885078</v>
+        <v>0.4337252570384458</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -740,10 +740,10 @@
         <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>14.72354656194007</v>
+        <v>15.92520679514612</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4337252570384458</v>
+        <v>0.4945554042885078</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -760,10 +760,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>16.49333370748002</v>
+        <v>15.41781746383798</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4989445773944082</v>
+        <v>0.4543805054829342</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -780,10 +780,10 @@
         <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>15.41781746383798</v>
+        <v>16.49333370748002</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4543805054829342</v>
+        <v>0.4989445773944082</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>

</xml_diff>